<commit_message>
map on tableau complete based on the data gathered from the class outlook files
</commit_message>
<xml_diff>
--- a/final_project_data(Excel).xlsx
+++ b/final_project_data(Excel).xlsx
@@ -9,16 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Distribution" sheetId="2" r:id="rId1"/>
     <sheet name="Mean No. of child Distribution" sheetId="4" r:id="rId2"/>
     <sheet name="final_project_data" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -989,11 +989,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>FERTILITY DISTRIBUTION AMONG MPS WITH RESPECT TO THEIR</a:t>
+              <a:t>FERTILITY DISTRIBUTION AMONG MPS GROUPED</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> POLITICAL PARTIES </a:t>
+              <a:t> BY POLITICAL PARTIES </a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1560,11 +1560,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1684073664"/>
-        <c:axId val="1684238224"/>
+        <c:axId val="-1532951664"/>
+        <c:axId val="-1532947296"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1684073664"/>
+        <c:axId val="-1532951664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1578,7 +1578,7 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:ln cap="sq">
+                    <a:ln>
                       <a:solidFill>
                         <a:srgbClr val="FF0000"/>
                       </a:solidFill>
@@ -1619,7 +1619,7 @@
             <a:p>
               <a:pPr>
                 <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:ln cap="sq">
+                  <a:ln>
                     <a:solidFill>
                       <a:srgbClr val="FF0000"/>
                     </a:solidFill>
@@ -1675,7 +1675,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1684238224"/>
+        <c:crossAx val="-1532947296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1683,7 +1683,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1684238224"/>
+        <c:axId val="-1532947296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1725,7 +1725,7 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:ln cap="sq">
+                    <a:ln>
                       <a:solidFill>
                         <a:srgbClr val="FF0000"/>
                       </a:solidFill>
@@ -1766,7 +1766,7 @@
             <a:p>
               <a:pPr>
                 <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:ln cap="sq">
+                  <a:ln>
                     <a:solidFill>
                       <a:srgbClr val="FF0000"/>
                     </a:solidFill>
@@ -1815,7 +1815,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1684073664"/>
+        <c:crossAx val="-1532951664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1844,7 +1844,7 @@
         <a:p>
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:ln cap="sq">
+              <a:ln>
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
@@ -1942,7 +1942,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>AVERAGE NUMBER OF CHILDREN OF MPs PER POLITICAL PARTY</a:t>
+              <a:t>AVERAGE NUMBER OF CHILDREN OF MPs PER POLITICAL PARTIES</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2055,11 +2055,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1793695552"/>
-        <c:axId val="1792886736"/>
+        <c:axId val="-1532911136"/>
+        <c:axId val="-1532907104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1793695552"/>
+        <c:axId val="-1532911136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2158,7 +2158,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1792886736"/>
+        <c:crossAx val="-1532907104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2166,7 +2166,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1792886736"/>
+        <c:axId val="-1532907104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2272,7 +2272,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1793695552"/>
+        <c:crossAx val="-1532911136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3411,16 +3411,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3446,16 +3446,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>901700</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4903,7 +4903,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:P10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField dataField="1" showAll="0"/>
@@ -5023,7 +5023,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
@@ -5360,8 +5360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W12" sqref="W12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AB11" sqref="AB11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5666,8 +5666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>